<commit_message>
insyallah sidang dapet nilai dan lulus
</commit_message>
<xml_diff>
--- a/new/excel.xlsx
+++ b/new/excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2325" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2325" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,9 +628,6 @@
   </si>
   <si>
     <t>informasi peranti waktu (HH:mm:ss)</t>
-  </si>
-  <si>
-    <t>qQi</t>
   </si>
   <si>
     <t>K1 &lt; K2</t>
@@ -729,6 +726,9 @@
       </rPr>
       <t>q</t>
     </r>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
@@ -1452,17 +1452,17 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1698,11 +1698,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-376148384"/>
-        <c:axId val="-380383088"/>
+        <c:axId val="1885393824"/>
+        <c:axId val="1885394912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-376148384"/>
+        <c:axId val="1885393824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1758,12 +1758,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-380383088"/>
+        <c:crossAx val="1885394912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-380383088"/>
+        <c:axId val="1885394912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1820,7 +1820,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-376148384"/>
+        <c:crossAx val="1885393824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5020,7 +5020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
@@ -5039,22 +5039,22 @@
         <v>119</v>
       </c>
       <c r="E3" s="88" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="87" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="G3" s="87" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="131" t="s">
+        <v>163</v>
+      </c>
+      <c r="I3" s="131" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" s="86" t="s">
         <v>161</v>
-      </c>
-      <c r="G3" s="87" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="133" t="s">
-        <v>164</v>
-      </c>
-      <c r="I3" s="133" t="s">
-        <v>152</v>
-      </c>
-      <c r="J3" s="86" t="s">
-        <v>162</v>
       </c>
       <c r="K3" s="87" t="s">
         <v>134</v>
@@ -5069,15 +5069,15 @@
         <v>133</v>
       </c>
       <c r="G4" s="85" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
+        <v>158</v>
+      </c>
+      <c r="H4" s="132"/>
+      <c r="I4" s="132"/>
       <c r="J4" s="90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K4" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.25">
@@ -5099,7 +5099,7 @@
       <c r="I5" s="129">
         <v>419</v>
       </c>
-      <c r="J5" s="131">
+      <c r="J5" s="133">
         <f>ABS(H5-I5)</f>
         <v>240</v>
       </c>
@@ -5121,7 +5121,7 @@
       <c r="G6" s="130"/>
       <c r="H6" s="130"/>
       <c r="I6" s="130"/>
-      <c r="J6" s="132"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="130"/>
       <c r="N6">
         <v>4</v>
@@ -5149,7 +5149,7 @@
       <c r="I7" s="129">
         <v>277</v>
       </c>
-      <c r="J7" s="131">
+      <c r="J7" s="133">
         <f t="shared" ref="J7" si="0">ABS(H7-I7)</f>
         <v>140</v>
       </c>
@@ -5171,7 +5171,7 @@
       <c r="G8" s="130"/>
       <c r="H8" s="130"/>
       <c r="I8" s="130"/>
-      <c r="J8" s="132"/>
+      <c r="J8" s="134"/>
       <c r="K8" s="130"/>
       <c r="N8">
         <v>2</v>
@@ -5196,7 +5196,7 @@
       <c r="I9" s="129">
         <v>103</v>
       </c>
-      <c r="J9" s="131">
+      <c r="J9" s="133">
         <f t="shared" ref="J9" si="1">ABS(H9-I9)</f>
         <v>264</v>
       </c>
@@ -5222,7 +5222,7 @@
       <c r="G10" s="130"/>
       <c r="H10" s="130"/>
       <c r="I10" s="130"/>
-      <c r="J10" s="132"/>
+      <c r="J10" s="134"/>
       <c r="K10" s="130"/>
       <c r="N10">
         <v>2</v>
@@ -5251,7 +5251,7 @@
       <c r="I11" s="129">
         <v>67</v>
       </c>
-      <c r="J11" s="131">
+      <c r="J11" s="133">
         <f t="shared" ref="J11" si="2">ABS(H11-I11)</f>
         <v>130</v>
       </c>
@@ -5273,7 +5273,7 @@
       <c r="G12" s="130"/>
       <c r="H12" s="130"/>
       <c r="I12" s="130"/>
-      <c r="J12" s="132"/>
+      <c r="J12" s="134"/>
       <c r="K12" s="130"/>
       <c r="N12">
         <v>2</v>
@@ -5298,7 +5298,7 @@
       <c r="I13" s="129">
         <v>31</v>
       </c>
-      <c r="J13" s="131">
+      <c r="J13" s="133">
         <f>ABS(H13-I13)</f>
         <v>106</v>
       </c>
@@ -5320,7 +5320,7 @@
       <c r="G14" s="130"/>
       <c r="H14" s="130"/>
       <c r="I14" s="130"/>
-      <c r="J14" s="132"/>
+      <c r="J14" s="134"/>
       <c r="K14" s="130"/>
       <c r="N14">
         <v>2</v>
@@ -5345,7 +5345,7 @@
       <c r="I15" s="129">
         <v>71</v>
       </c>
-      <c r="J15" s="131">
+      <c r="J15" s="133">
         <f t="shared" ref="J15" si="3">ABS(H15-I15)</f>
         <v>39</v>
       </c>
@@ -5367,7 +5367,7 @@
       <c r="G16" s="130"/>
       <c r="H16" s="130"/>
       <c r="I16" s="130"/>
-      <c r="J16" s="132"/>
+      <c r="J16" s="134"/>
       <c r="K16" s="130"/>
       <c r="N16">
         <v>2</v>
@@ -5392,7 +5392,7 @@
       <c r="I17" s="129">
         <v>479</v>
       </c>
-      <c r="J17" s="131">
+      <c r="J17" s="133">
         <f t="shared" ref="J17" si="4">ABS(H17-I17)</f>
         <v>132</v>
       </c>
@@ -5414,7 +5414,7 @@
       <c r="G18" s="130"/>
       <c r="H18" s="130"/>
       <c r="I18" s="130"/>
-      <c r="J18" s="132"/>
+      <c r="J18" s="134"/>
       <c r="K18" s="130"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
@@ -5436,7 +5436,7 @@
       <c r="I19" s="129">
         <v>47</v>
       </c>
-      <c r="J19" s="131">
+      <c r="J19" s="133">
         <f t="shared" ref="J19" si="5">ABS(H19-I19)</f>
         <v>90</v>
       </c>
@@ -5455,7 +5455,7 @@
       <c r="G20" s="130"/>
       <c r="H20" s="130"/>
       <c r="I20" s="130"/>
-      <c r="J20" s="132"/>
+      <c r="J20" s="134"/>
       <c r="K20" s="130"/>
     </row>
     <row r="21" spans="4:14" x14ac:dyDescent="0.25">
@@ -5477,7 +5477,7 @@
       <c r="I21" s="129">
         <v>149</v>
       </c>
-      <c r="J21" s="131">
+      <c r="J21" s="133">
         <f>ABS(H21-I21)</f>
         <v>290</v>
       </c>
@@ -5496,7 +5496,7 @@
       <c r="G22" s="130"/>
       <c r="H22" s="130"/>
       <c r="I22" s="130"/>
-      <c r="J22" s="132"/>
+      <c r="J22" s="134"/>
       <c r="K22" s="130"/>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
@@ -5518,7 +5518,7 @@
       <c r="I23" s="129">
         <v>257</v>
       </c>
-      <c r="J23" s="131">
+      <c r="J23" s="133">
         <f t="shared" ref="J23" si="6">ABS(H23-I23)</f>
         <v>110</v>
       </c>
@@ -5537,7 +5537,7 @@
       <c r="G24" s="130"/>
       <c r="H24" s="130"/>
       <c r="I24" s="130"/>
-      <c r="J24" s="132"/>
+      <c r="J24" s="134"/>
       <c r="K24" s="130"/>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.25">
@@ -5559,7 +5559,7 @@
       <c r="I25" s="129">
         <v>379</v>
       </c>
-      <c r="J25" s="131">
+      <c r="J25" s="133">
         <f t="shared" ref="J25" si="7">ABS(H25-I25)</f>
         <v>200</v>
       </c>
@@ -5578,7 +5578,7 @@
       <c r="G26" s="130"/>
       <c r="H26" s="130"/>
       <c r="I26" s="130"/>
-      <c r="J26" s="132"/>
+      <c r="J26" s="134"/>
       <c r="K26" s="130"/>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.25">
@@ -5600,7 +5600,7 @@
       <c r="I27" s="129">
         <v>499</v>
       </c>
-      <c r="J27" s="131">
+      <c r="J27" s="133">
         <f t="shared" ref="J27" si="8">ABS(H27-I27)</f>
         <v>38</v>
       </c>
@@ -5619,7 +5619,7 @@
       <c r="G28" s="130"/>
       <c r="H28" s="130"/>
       <c r="I28" s="130"/>
-      <c r="J28" s="132"/>
+      <c r="J28" s="134"/>
       <c r="K28" s="130"/>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.25">
@@ -5641,7 +5641,7 @@
       <c r="I29" s="129">
         <v>61</v>
       </c>
-      <c r="J29" s="131">
+      <c r="J29" s="133">
         <f>ABS(H29-I29)</f>
         <v>38</v>
       </c>
@@ -5660,7 +5660,7 @@
       <c r="G30" s="130"/>
       <c r="H30" s="130"/>
       <c r="I30" s="130"/>
-      <c r="J30" s="132"/>
+      <c r="J30" s="134"/>
       <c r="K30" s="130"/>
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.25">
@@ -5745,6 +5745,83 @@
     </row>
   </sheetData>
   <mergeCells count="101">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="K35:K36"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
@@ -5765,87 +5842,10 @@
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="H31:H32"/>
     <mergeCell ref="I31:I32"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K29:K30"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="I23:I24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5858,7 +5858,7 @@
   <dimension ref="D4:M33"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6108,8 +6108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="D5:G12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6167,13 +6167,13 @@
     </row>
     <row r="9" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="70" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="E9" s="30">
         <v>10</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G9" s="75" t="b">
         <v>0</v>
@@ -6186,13 +6186,13 @@
     </row>
     <row r="10" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="79" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="E10" s="78">
         <v>80</v>
       </c>
       <c r="F10" s="80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G10" s="81" t="b">
         <f>E$9&lt; E10</f>
@@ -6213,7 +6213,7 @@
       <c r="D12" s="138"/>
       <c r="E12" s="139"/>
       <c r="F12" s="84" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G12" s="83">
         <v>419</v>

</xml_diff>

<commit_message>
bismillah print kumpul selesai semua insyallah
</commit_message>
<xml_diff>
--- a/new/excel.xlsx
+++ b/new/excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2325" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9195" windowHeight="2325" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sheet10" sheetId="12" r:id="rId7"/>
     <sheet name="1new" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet6" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="193">
   <si>
     <t xml:space="preserve">        &lt;item&gt;GMT-1&lt;/item&gt; </t>
   </si>
@@ -779,6 +780,15 @@
       </rPr>
       <t xml:space="preserve"> informasi peranti waktu</t>
     </r>
+  </si>
+  <si>
+    <t>Hasil Enkripsi Teks 4</t>
+  </si>
+  <si>
+    <t>p dan q default</t>
+  </si>
+  <si>
+    <t>p dan q base informasi peranti</t>
   </si>
 </sst>
 </file>
@@ -928,7 +938,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1196,11 +1206,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1478,6 +1501,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1562,6 +1589,33 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1580,32 +1634,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1667,19 +1703,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1742,7 +1776,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1845,11 +1878,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="101624480"/>
-        <c:axId val="101622848"/>
+        <c:axId val="1627619024"/>
+        <c:axId val="1627616304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101624480"/>
+        <c:axId val="1627619024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,12 +1938,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101622848"/>
+        <c:crossAx val="1627616304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101622848"/>
+        <c:axId val="1627616304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +2000,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101624480"/>
+        <c:crossAx val="1627619024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2258,11 +2291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="332840768"/>
-        <c:axId val="332838592"/>
+        <c:axId val="1627619568"/>
+        <c:axId val="1627621200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332840768"/>
+        <c:axId val="1627619568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332838592"/>
+        <c:crossAx val="1627621200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2313,7 +2346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332838592"/>
+        <c:axId val="1627621200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2364,7 +2397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332840768"/>
+        <c:crossAx val="1627619568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4094,42 +4127,42 @@
   <sheetData>
     <row r="2" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="121" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="121"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="123"/>
     </row>
     <row r="4" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="122"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
-      <c r="I4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="126"/>
     </row>
     <row r="5" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D5" s="115" t="s">
+      <c r="D5" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="116"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="55"/>
       <c r="G5" s="56"/>
-      <c r="H5" s="115" t="s">
+      <c r="H5" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="116"/>
+      <c r="I5" s="118"/>
     </row>
     <row r="6" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="117"/>
-      <c r="E6" s="118"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="120"/>
       <c r="F6" s="55"/>
       <c r="G6" s="56"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="120"/>
     </row>
     <row r="7" spans="4:18" x14ac:dyDescent="0.25">
       <c r="D7" s="57" t="s">
@@ -4355,6 +4388,155 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="D3:E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="55.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="186" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="187" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D4" s="186" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="187" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="185" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="166" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="162"/>
+      <c r="E6" s="163"/>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="162"/>
+      <c r="E7" s="163"/>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="162"/>
+      <c r="E8" s="163"/>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="162"/>
+      <c r="E9" s="163"/>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="162"/>
+      <c r="E11" s="163"/>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="162"/>
+      <c r="E12" s="163"/>
+    </row>
+    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="162"/>
+      <c r="E13" s="163"/>
+    </row>
+    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="162"/>
+      <c r="E14" s="163"/>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="162"/>
+      <c r="E15" s="163"/>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="162"/>
+      <c r="E16" s="163"/>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="162"/>
+      <c r="E17" s="163"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="162"/>
+      <c r="E18" s="163"/>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="162"/>
+      <c r="E19" s="163"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="162"/>
+      <c r="E20" s="163"/>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="162"/>
+      <c r="E21" s="163"/>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="162"/>
+      <c r="E22" s="163"/>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="162"/>
+      <c r="E23" s="163"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="162"/>
+      <c r="E24" s="163"/>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="162"/>
+      <c r="E25" s="163"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="184"/>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="184"/>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="184"/>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="184"/>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="184"/>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="184"/>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="183"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E5:E25"/>
+    <mergeCell ref="D5:D25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4390,23 +4572,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
     </row>
     <row r="2" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="127" t="s">
+      <c r="D2" s="129" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="129"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="131"/>
       <c r="I2" s="32"/>
       <c r="M2" s="24">
         <v>4814863028233940</v>
@@ -4487,13 +4669,13 @@
       <c r="C9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="125" t="s">
+      <c r="D9" s="127" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="140"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="126"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="142"/>
+      <c r="H9" s="128"/>
       <c r="M9" t="s">
         <v>94</v>
       </c>
@@ -4758,26 +4940,26 @@
       <c r="C21" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="138"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="138"/>
-      <c r="H21" s="139"/>
+      <c r="E21" s="140"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="140"/>
+      <c r="H21" s="141"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="137" t="s">
+      <c r="D22" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="138"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="138"/>
-      <c r="H22" s="139"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="141"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
@@ -4854,25 +5036,25 @@
       <c r="C48" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="130" t="s">
+      <c r="D48" s="132" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="131"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="132"/>
+      <c r="E48" s="133"/>
+      <c r="F48" s="133"/>
+      <c r="G48" s="133"/>
+      <c r="H48" s="134"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="133" t="s">
+      <c r="D49" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="134"/>
-      <c r="F49" s="134"/>
-      <c r="G49" s="134"/>
-      <c r="H49" s="135"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="136"/>
+      <c r="H49" s="137"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="4" t="s">
@@ -5160,10 +5342,10 @@
       </c>
     </row>
     <row r="75" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F75" s="125" t="s">
+      <c r="F75" s="127" t="s">
         <v>118</v>
       </c>
-      <c r="G75" s="126"/>
+      <c r="G75" s="128"/>
       <c r="H75" s="38">
         <f>AVERAGE(H70:H74)</f>
         <v>120.4</v>
@@ -6187,7 +6369,7 @@
     </row>
     <row r="2" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="143" t="s">
         <v>119</v>
       </c>
       <c r="E3" s="80" t="s">
@@ -6199,32 +6381,32 @@
       <c r="G3" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="H3" s="156" t="s">
+      <c r="H3" s="152" t="s">
         <v>155</v>
       </c>
-      <c r="I3" s="156" t="s">
+      <c r="I3" s="152" t="s">
         <v>147</v>
       </c>
-      <c r="J3" s="151" t="s">
+      <c r="J3" s="147" t="s">
         <v>158</v>
       </c>
-      <c r="K3" s="152"/>
-      <c r="M3" s="141" t="s">
+      <c r="K3" s="148"/>
+      <c r="M3" s="143" t="s">
         <v>119</v>
       </c>
-      <c r="N3" s="156" t="s">
+      <c r="N3" s="152" t="s">
         <v>155</v>
       </c>
-      <c r="O3" s="156" t="s">
+      <c r="O3" s="152" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="151" t="s">
+      <c r="P3" s="147" t="s">
         <v>158</v>
       </c>
-      <c r="Q3" s="152"/>
+      <c r="Q3" s="148"/>
     </row>
     <row r="4" spans="4:17" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="142"/>
+      <c r="D4" s="144"/>
       <c r="E4" s="67" t="s">
         <v>132</v>
       </c>
@@ -6234,17 +6416,17 @@
       <c r="G4" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="157"/>
-      <c r="I4" s="157"/>
+      <c r="H4" s="153"/>
+      <c r="I4" s="153"/>
       <c r="J4" s="89" t="s">
         <v>157</v>
       </c>
       <c r="K4" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="M4" s="142"/>
-      <c r="N4" s="157"/>
-      <c r="O4" s="157"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="153"/>
+      <c r="O4" s="153"/>
       <c r="P4" s="89" t="s">
         <v>157</v>
       </c>
@@ -6253,7 +6435,7 @@
       </c>
     </row>
     <row r="5" spans="4:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="141">
+      <c r="D5" s="143">
         <v>1</v>
       </c>
       <c r="E5" s="53">
@@ -6262,58 +6444,58 @@
       <c r="F5" s="54">
         <v>0.2854976851851852</v>
       </c>
-      <c r="G5" s="141">
+      <c r="G5" s="143">
         <v>5</v>
       </c>
-      <c r="H5" s="141">
+      <c r="H5" s="143">
         <v>97</v>
       </c>
-      <c r="I5" s="141">
+      <c r="I5" s="143">
         <v>167</v>
       </c>
-      <c r="J5" s="149">
+      <c r="J5" s="145">
         <v>121</v>
       </c>
-      <c r="K5" s="141">
+      <c r="K5" s="143">
         <v>4873</v>
       </c>
-      <c r="M5" s="141">
+      <c r="M5" s="143">
         <v>1</v>
       </c>
-      <c r="N5" s="141">
+      <c r="N5" s="143">
         <v>61</v>
       </c>
-      <c r="O5" s="141">
+      <c r="O5" s="143">
         <v>227</v>
       </c>
-      <c r="P5" s="149">
+      <c r="P5" s="145">
         <v>191</v>
       </c>
-      <c r="Q5" s="141">
+      <c r="Q5" s="143">
         <v>13631</v>
       </c>
     </row>
     <row r="6" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="142"/>
+      <c r="D6" s="144"/>
       <c r="E6" s="67" t="s">
         <v>134</v>
       </c>
       <c r="F6" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="142"/>
-      <c r="H6" s="142"/>
-      <c r="I6" s="142"/>
-      <c r="J6" s="150"/>
-      <c r="K6" s="142"/>
-      <c r="M6" s="142"/>
-      <c r="N6" s="142"/>
-      <c r="O6" s="142"/>
-      <c r="P6" s="150"/>
-      <c r="Q6" s="142"/>
+      <c r="G6" s="144"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="144"/>
+      <c r="M6" s="144"/>
+      <c r="N6" s="144"/>
+      <c r="O6" s="144"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="144"/>
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D7" s="141">
+      <c r="D7" s="143">
         <v>2</v>
       </c>
       <c r="E7" s="84">
@@ -6322,58 +6504,58 @@
       <c r="F7" s="83">
         <v>0.12224537037037037</v>
       </c>
-      <c r="G7" s="141">
+      <c r="G7" s="143">
         <v>1</v>
       </c>
-      <c r="H7" s="141">
+      <c r="H7" s="143">
         <v>23</v>
       </c>
-      <c r="I7" s="141">
+      <c r="I7" s="143">
         <v>167</v>
       </c>
-      <c r="J7" s="149">
+      <c r="J7" s="145">
         <v>89</v>
       </c>
-      <c r="K7" s="141">
+      <c r="K7" s="143">
         <v>2421</v>
       </c>
-      <c r="M7" s="141">
+      <c r="M7" s="143">
         <v>2</v>
       </c>
-      <c r="N7" s="141">
+      <c r="N7" s="143">
         <v>53</v>
       </c>
-      <c r="O7" s="141">
+      <c r="O7" s="143">
         <v>331</v>
       </c>
-      <c r="P7" s="149">
+      <c r="P7" s="145">
         <v>301</v>
       </c>
-      <c r="Q7" s="141">
+      <c r="Q7" s="143">
         <v>5701</v>
       </c>
     </row>
     <row r="8" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="142"/>
+      <c r="D8" s="144"/>
       <c r="E8" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F8" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="142"/>
-      <c r="H8" s="142"/>
-      <c r="I8" s="142"/>
-      <c r="J8" s="150"/>
-      <c r="K8" s="142"/>
-      <c r="M8" s="142"/>
-      <c r="N8" s="142"/>
-      <c r="O8" s="142"/>
-      <c r="P8" s="150"/>
-      <c r="Q8" s="142"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="144"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="144"/>
+      <c r="M8" s="144"/>
+      <c r="N8" s="144"/>
+      <c r="O8" s="144"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="144"/>
     </row>
     <row r="9" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D9" s="141">
+      <c r="D9" s="143">
         <v>3</v>
       </c>
       <c r="E9" s="84">
@@ -6382,58 +6564,58 @@
       <c r="F9" s="83">
         <v>0.1257175925925926</v>
       </c>
-      <c r="G9" s="141">
+      <c r="G9" s="143">
         <v>1</v>
       </c>
-      <c r="H9" s="141">
+      <c r="H9" s="143">
         <v>41</v>
       </c>
-      <c r="I9" s="141">
+      <c r="I9" s="143">
         <v>23</v>
       </c>
-      <c r="J9" s="149">
+      <c r="J9" s="145">
         <v>27</v>
       </c>
-      <c r="K9" s="141">
+      <c r="K9" s="143">
         <v>163</v>
       </c>
-      <c r="M9" s="141">
+      <c r="M9" s="143">
         <v>3</v>
       </c>
-      <c r="N9" s="141">
+      <c r="N9" s="143">
         <v>89</v>
       </c>
-      <c r="O9" s="141">
+      <c r="O9" s="143">
         <v>409</v>
       </c>
-      <c r="P9" s="149">
+      <c r="P9" s="145">
         <v>281</v>
       </c>
-      <c r="Q9" s="141">
+      <c r="Q9" s="143">
         <v>12905</v>
       </c>
     </row>
     <row r="10" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="142"/>
+      <c r="D10" s="144"/>
       <c r="E10" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="142"/>
-      <c r="J10" s="150"/>
-      <c r="K10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="150"/>
-      <c r="Q10" s="142"/>
+      <c r="G10" s="144"/>
+      <c r="H10" s="144"/>
+      <c r="I10" s="144"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="144"/>
+      <c r="M10" s="144"/>
+      <c r="N10" s="144"/>
+      <c r="O10" s="144"/>
+      <c r="P10" s="146"/>
+      <c r="Q10" s="144"/>
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D11" s="141">
+      <c r="D11" s="143">
         <v>4</v>
       </c>
       <c r="E11" s="84">
@@ -6442,58 +6624,58 @@
       <c r="F11" s="83">
         <v>0.5875231481481481</v>
       </c>
-      <c r="G11" s="141">
+      <c r="G11" s="143">
         <v>21</v>
       </c>
-      <c r="H11" s="141">
+      <c r="H11" s="143">
         <v>269</v>
       </c>
-      <c r="I11" s="141">
+      <c r="I11" s="143">
         <v>137</v>
       </c>
-      <c r="J11" s="149">
+      <c r="J11" s="145">
         <v>73</v>
       </c>
-      <c r="K11" s="141">
+      <c r="K11" s="143">
         <v>32953</v>
       </c>
-      <c r="M11" s="141">
+      <c r="M11" s="143">
         <v>4</v>
       </c>
-      <c r="N11" s="141">
+      <c r="N11" s="143">
         <v>257</v>
       </c>
-      <c r="O11" s="141">
+      <c r="O11" s="143">
         <v>137</v>
       </c>
-      <c r="P11" s="149">
+      <c r="P11" s="145">
         <v>71</v>
       </c>
-      <c r="Q11" s="141">
+      <c r="Q11" s="143">
         <v>14711</v>
       </c>
     </row>
     <row r="12" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="142"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F12" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="142"/>
-      <c r="H12" s="142"/>
-      <c r="I12" s="142"/>
-      <c r="J12" s="150"/>
-      <c r="K12" s="142"/>
-      <c r="M12" s="142"/>
-      <c r="N12" s="142"/>
-      <c r="O12" s="142"/>
-      <c r="P12" s="150"/>
-      <c r="Q12" s="142"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="144"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="144"/>
+      <c r="M12" s="144"/>
+      <c r="N12" s="144"/>
+      <c r="O12" s="144"/>
+      <c r="P12" s="146"/>
+      <c r="Q12" s="144"/>
     </row>
     <row r="13" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D13" s="141">
+      <c r="D13" s="143">
         <v>5</v>
       </c>
       <c r="E13" s="84">
@@ -6502,58 +6684,58 @@
       <c r="F13" s="86">
         <v>0.25766203703703705</v>
       </c>
-      <c r="G13" s="141">
+      <c r="G13" s="143">
         <v>4</v>
       </c>
-      <c r="H13" s="141">
+      <c r="H13" s="143">
         <v>97</v>
       </c>
-      <c r="I13" s="141">
+      <c r="I13" s="143">
         <v>241</v>
       </c>
-      <c r="J13" s="149">
+      <c r="J13" s="145">
         <v>199</v>
       </c>
-      <c r="K13" s="141">
+      <c r="K13" s="143">
         <v>10999</v>
       </c>
-      <c r="M13" s="141">
+      <c r="M13" s="143">
         <v>5</v>
       </c>
-      <c r="N13" s="141">
+      <c r="N13" s="143">
         <v>61</v>
       </c>
-      <c r="O13" s="141">
+      <c r="O13" s="143">
         <v>113</v>
       </c>
-      <c r="P13" s="149">
+      <c r="P13" s="145">
         <v>137</v>
       </c>
-      <c r="Q13" s="141">
+      <c r="Q13" s="143">
         <v>1913</v>
       </c>
     </row>
     <row r="14" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="142"/>
+      <c r="D14" s="144"/>
       <c r="E14" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F14" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="142"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="142"/>
-      <c r="J14" s="150"/>
-      <c r="K14" s="142"/>
-      <c r="M14" s="142"/>
-      <c r="N14" s="142"/>
-      <c r="O14" s="142"/>
-      <c r="P14" s="150"/>
-      <c r="Q14" s="142"/>
+      <c r="G14" s="144"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="144"/>
+      <c r="J14" s="146"/>
+      <c r="K14" s="144"/>
+      <c r="M14" s="144"/>
+      <c r="N14" s="144"/>
+      <c r="O14" s="144"/>
+      <c r="P14" s="146"/>
+      <c r="Q14" s="144"/>
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D15" s="141">
+      <c r="D15" s="143">
         <v>6</v>
       </c>
       <c r="E15" s="84">
@@ -6562,58 +6744,58 @@
       <c r="F15" s="86">
         <v>0.51113425925925926</v>
       </c>
-      <c r="G15" s="141">
+      <c r="G15" s="143">
         <v>23</v>
       </c>
-      <c r="H15" s="141">
+      <c r="H15" s="143">
         <v>227</v>
       </c>
-      <c r="I15" s="141">
+      <c r="I15" s="143">
         <v>367</v>
       </c>
-      <c r="J15" s="149">
+      <c r="J15" s="145">
         <v>227</v>
       </c>
-      <c r="K15" s="141">
+      <c r="K15" s="143">
         <v>17855</v>
       </c>
-      <c r="M15" s="141">
+      <c r="M15" s="143">
         <v>6</v>
       </c>
-      <c r="N15" s="141">
+      <c r="N15" s="143">
         <v>229</v>
       </c>
-      <c r="O15" s="141">
+      <c r="O15" s="143">
         <v>211</v>
       </c>
-      <c r="P15" s="149">
+      <c r="P15" s="145">
         <v>221</v>
       </c>
-      <c r="Q15" s="141">
+      <c r="Q15" s="143">
         <v>33581</v>
       </c>
     </row>
     <row r="16" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="142"/>
+      <c r="D16" s="144"/>
       <c r="E16" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F16" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="150"/>
-      <c r="K16" s="142"/>
-      <c r="M16" s="142"/>
-      <c r="N16" s="142"/>
-      <c r="O16" s="142"/>
-      <c r="P16" s="150"/>
-      <c r="Q16" s="142"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="146"/>
+      <c r="K16" s="144"/>
+      <c r="M16" s="144"/>
+      <c r="N16" s="144"/>
+      <c r="O16" s="144"/>
+      <c r="P16" s="146"/>
+      <c r="Q16" s="144"/>
     </row>
     <row r="17" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D17" s="141">
+      <c r="D17" s="143">
         <v>7</v>
       </c>
       <c r="E17" s="84">
@@ -6622,58 +6804,58 @@
       <c r="F17" s="86">
         <v>0.76460648148148147</v>
       </c>
-      <c r="G17" s="141">
+      <c r="G17" s="143">
         <v>17</v>
       </c>
-      <c r="H17" s="141">
+      <c r="H17" s="143">
         <v>367</v>
       </c>
-      <c r="I17" s="141">
+      <c r="I17" s="143">
         <v>487</v>
       </c>
-      <c r="J17" s="149">
+      <c r="J17" s="145">
         <v>283</v>
       </c>
-      <c r="K17" s="141">
+      <c r="K17" s="143">
         <v>143935</v>
       </c>
-      <c r="M17" s="141">
+      <c r="M17" s="143">
         <v>7</v>
       </c>
-      <c r="N17" s="141">
+      <c r="N17" s="143">
         <v>113</v>
       </c>
-      <c r="O17" s="141">
+      <c r="O17" s="143">
         <v>2</v>
       </c>
-      <c r="P17" s="149">
+      <c r="P17" s="145">
         <v>3</v>
       </c>
-      <c r="Q17" s="141">
+      <c r="Q17" s="143">
         <v>187</v>
       </c>
     </row>
     <row r="18" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="142"/>
+      <c r="D18" s="144"/>
       <c r="E18" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F18" s="85" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="142"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="150"/>
-      <c r="K18" s="142"/>
-      <c r="M18" s="142"/>
-      <c r="N18" s="142"/>
-      <c r="O18" s="142"/>
-      <c r="P18" s="150"/>
-      <c r="Q18" s="142"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="144"/>
+      <c r="M18" s="144"/>
+      <c r="N18" s="144"/>
+      <c r="O18" s="144"/>
+      <c r="P18" s="146"/>
+      <c r="Q18" s="144"/>
     </row>
     <row r="19" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D19" s="141">
+      <c r="D19" s="143">
         <v>8</v>
       </c>
       <c r="E19" s="84">
@@ -6682,61 +6864,61 @@
       <c r="F19" s="83">
         <v>0.60141203703703705</v>
       </c>
-      <c r="G19" s="141">
+      <c r="G19" s="143">
         <v>21</v>
       </c>
-      <c r="H19" s="141">
+      <c r="H19" s="143">
         <v>269</v>
       </c>
-      <c r="I19" s="141">
+      <c r="I19" s="143">
         <v>53</v>
       </c>
-      <c r="J19" s="149">
+      <c r="J19" s="145">
         <v>35</v>
       </c>
-      <c r="K19" s="141">
+      <c r="K19" s="143">
         <v>11547</v>
       </c>
-      <c r="M19" s="141">
+      <c r="M19" s="143">
         <v>8</v>
       </c>
-      <c r="N19" s="141">
+      <c r="N19" s="143">
         <v>83</v>
       </c>
-      <c r="O19" s="141">
+      <c r="O19" s="143">
         <v>139</v>
       </c>
-      <c r="P19" s="149">
+      <c r="P19" s="145">
         <v>109</v>
       </c>
-      <c r="Q19" s="141">
+      <c r="Q19" s="143">
         <v>6229</v>
       </c>
     </row>
     <row r="20" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="142"/>
+      <c r="D20" s="144"/>
       <c r="E20" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F20" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="142"/>
-      <c r="H20" s="142"/>
-      <c r="I20" s="142"/>
-      <c r="J20" s="150"/>
-      <c r="K20" s="142"/>
-      <c r="M20" s="142"/>
-      <c r="N20" s="142"/>
-      <c r="O20" s="142"/>
-      <c r="P20" s="150"/>
-      <c r="Q20" s="142"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="146"/>
+      <c r="K20" s="144"/>
+      <c r="M20" s="144"/>
+      <c r="N20" s="144"/>
+      <c r="O20" s="144"/>
+      <c r="P20" s="146"/>
+      <c r="Q20" s="144"/>
       <c r="R20">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D21" s="141">
+      <c r="D21" s="143">
         <v>9</v>
       </c>
       <c r="E21" s="84">
@@ -6745,34 +6927,34 @@
       <c r="F21" s="86">
         <v>0.56321759259259263</v>
       </c>
-      <c r="G21" s="141">
+      <c r="G21" s="143">
         <v>22</v>
       </c>
-      <c r="H21" s="141">
+      <c r="H21" s="143">
         <v>241</v>
       </c>
-      <c r="I21" s="141">
+      <c r="I21" s="143">
         <v>151</v>
       </c>
-      <c r="J21" s="149">
+      <c r="J21" s="145">
         <v>137</v>
       </c>
-      <c r="K21" s="141">
+      <c r="K21" s="143">
         <v>22073</v>
       </c>
-      <c r="M21" s="141">
+      <c r="M21" s="143">
         <v>9</v>
       </c>
-      <c r="N21" s="141">
+      <c r="N21" s="143">
         <v>7</v>
       </c>
-      <c r="O21" s="141">
+      <c r="O21" s="143">
         <v>173</v>
       </c>
-      <c r="P21" s="149">
+      <c r="P21" s="145">
         <v>125</v>
       </c>
-      <c r="Q21" s="141">
+      <c r="Q21" s="143">
         <v>677</v>
       </c>
       <c r="R21">
@@ -6780,26 +6962,26 @@
       </c>
     </row>
     <row r="22" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="142"/>
+      <c r="D22" s="144"/>
       <c r="E22" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F22" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="142"/>
-      <c r="H22" s="142"/>
-      <c r="I22" s="142"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="142"/>
-      <c r="M22" s="142"/>
-      <c r="N22" s="142"/>
-      <c r="O22" s="142"/>
-      <c r="P22" s="150"/>
-      <c r="Q22" s="142"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="144"/>
+      <c r="I22" s="144"/>
+      <c r="J22" s="146"/>
+      <c r="K22" s="144"/>
+      <c r="M22" s="144"/>
+      <c r="N22" s="144"/>
+      <c r="O22" s="144"/>
+      <c r="P22" s="146"/>
+      <c r="Q22" s="144"/>
     </row>
     <row r="23" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D23" s="141">
+      <c r="D23" s="143">
         <v>10</v>
       </c>
       <c r="E23" s="84">
@@ -6808,62 +6990,62 @@
       <c r="F23" s="83">
         <v>0.19168981481481481</v>
       </c>
-      <c r="G23" s="141">
+      <c r="G23" s="143">
         <v>2</v>
       </c>
-      <c r="H23" s="141">
+      <c r="H23" s="143">
         <v>59</v>
       </c>
-      <c r="I23" s="141">
+      <c r="I23" s="143">
         <v>263</v>
       </c>
-      <c r="J23" s="149">
+      <c r="J23" s="145">
         <v>117</v>
       </c>
-      <c r="K23" s="141">
+      <c r="K23" s="143">
         <v>11949</v>
       </c>
-      <c r="M23" s="141">
+      <c r="M23" s="143">
         <v>10</v>
       </c>
-      <c r="N23" s="141">
+      <c r="N23" s="143">
         <v>127</v>
       </c>
-      <c r="O23" s="141">
+      <c r="O23" s="143">
         <v>389</v>
       </c>
-      <c r="P23" s="149">
+      <c r="P23" s="145">
         <v>275</v>
       </c>
-      <c r="Q23" s="141">
+      <c r="Q23" s="143">
         <v>30755</v>
       </c>
     </row>
     <row r="24" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="142"/>
+      <c r="D24" s="144"/>
       <c r="E24" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F24" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="142"/>
-      <c r="H24" s="142"/>
-      <c r="I24" s="142"/>
-      <c r="J24" s="150"/>
-      <c r="K24" s="142"/>
-      <c r="M24" s="142"/>
-      <c r="N24" s="142"/>
-      <c r="O24" s="142"/>
-      <c r="P24" s="150"/>
-      <c r="Q24" s="142"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="144"/>
+      <c r="M24" s="144"/>
+      <c r="N24" s="144"/>
+      <c r="O24" s="144"/>
+      <c r="P24" s="146"/>
+      <c r="Q24" s="144"/>
       <c r="R24">
         <f>R20+R21</f>
         <v>7.83</v>
       </c>
     </row>
     <row r="25" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D25" s="141">
+      <c r="D25" s="143">
         <v>11</v>
       </c>
       <c r="E25" s="84">
@@ -6872,34 +7054,34 @@
       <c r="F25" s="86">
         <v>0.65349537037037042</v>
       </c>
-      <c r="G25" s="141">
+      <c r="G25" s="143">
         <v>20</v>
       </c>
-      <c r="H25" s="141">
+      <c r="H25" s="143">
         <v>283</v>
       </c>
-      <c r="I25" s="141">
+      <c r="I25" s="143">
         <v>383</v>
       </c>
-      <c r="J25" s="149">
+      <c r="J25" s="145">
         <v>239</v>
       </c>
-      <c r="K25" s="141">
+      <c r="K25" s="143">
         <v>51383</v>
       </c>
-      <c r="M25" s="141">
+      <c r="M25" s="143">
         <v>11</v>
       </c>
-      <c r="N25" s="141">
+      <c r="N25" s="143">
         <v>97</v>
       </c>
-      <c r="O25" s="141">
+      <c r="O25" s="143">
         <v>401</v>
       </c>
-      <c r="P25" s="149">
+      <c r="P25" s="145">
         <v>299</v>
       </c>
-      <c r="Q25" s="141">
+      <c r="Q25" s="143">
         <v>899</v>
       </c>
       <c r="R25">
@@ -6908,26 +7090,26 @@
       </c>
     </row>
     <row r="26" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="142"/>
+      <c r="D26" s="144"/>
       <c r="E26" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F26" s="85" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="142"/>
-      <c r="H26" s="142"/>
-      <c r="I26" s="142"/>
-      <c r="J26" s="150"/>
-      <c r="K26" s="142"/>
-      <c r="M26" s="142"/>
-      <c r="N26" s="142"/>
-      <c r="O26" s="142"/>
-      <c r="P26" s="150"/>
-      <c r="Q26" s="142"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="146"/>
+      <c r="K26" s="144"/>
+      <c r="M26" s="144"/>
+      <c r="N26" s="144"/>
+      <c r="O26" s="144"/>
+      <c r="P26" s="146"/>
+      <c r="Q26" s="144"/>
     </row>
     <row r="27" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D27" s="141">
+      <c r="D27" s="143">
         <v>12</v>
       </c>
       <c r="E27" s="84">
@@ -6936,74 +7118,74 @@
       <c r="F27" s="83">
         <v>0.49030092592592589</v>
       </c>
-      <c r="G27" s="141">
+      <c r="G27" s="143">
         <v>9</v>
       </c>
-      <c r="H27" s="141">
+      <c r="H27" s="143">
         <v>197</v>
       </c>
-      <c r="I27" s="141">
+      <c r="I27" s="143">
         <v>503</v>
       </c>
-      <c r="J27" s="149">
+      <c r="J27" s="145">
         <v>225</v>
       </c>
-      <c r="K27" s="141">
+      <c r="K27" s="143">
         <v>20553</v>
       </c>
-      <c r="M27" s="141">
+      <c r="M27" s="143">
         <v>12</v>
       </c>
-      <c r="N27" s="141">
+      <c r="N27" s="143">
         <v>71</v>
       </c>
-      <c r="O27" s="141">
+      <c r="O27" s="143">
         <v>53</v>
       </c>
-      <c r="P27" s="149">
+      <c r="P27" s="145">
         <v>53</v>
       </c>
-      <c r="Q27" s="141">
+      <c r="Q27" s="143">
         <v>1717</v>
       </c>
     </row>
     <row r="28" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="142"/>
+      <c r="D28" s="144"/>
       <c r="E28" s="81" t="s">
         <v>135</v>
       </c>
       <c r="F28" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="G28" s="142"/>
-      <c r="H28" s="142"/>
-      <c r="I28" s="142"/>
-      <c r="J28" s="150"/>
-      <c r="K28" s="142"/>
-      <c r="M28" s="142"/>
-      <c r="N28" s="142"/>
-      <c r="O28" s="142"/>
-      <c r="P28" s="150"/>
-      <c r="Q28" s="142"/>
+      <c r="G28" s="144"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="144"/>
+      <c r="J28" s="146"/>
+      <c r="K28" s="144"/>
+      <c r="M28" s="144"/>
+      <c r="N28" s="144"/>
+      <c r="O28" s="144"/>
+      <c r="P28" s="146"/>
+      <c r="Q28" s="144"/>
     </row>
     <row r="29" spans="4:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="153" t="s">
+      <c r="D29" s="149" t="s">
         <v>170</v>
       </c>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="154"/>
-      <c r="I29" s="154"/>
-      <c r="J29" s="154"/>
-      <c r="K29" s="155"/>
-      <c r="M29" s="143" t="s">
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
+      <c r="G29" s="150"/>
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="151"/>
+      <c r="M29" s="154" t="s">
         <v>170</v>
       </c>
-      <c r="N29" s="144"/>
-      <c r="O29" s="144"/>
-      <c r="P29" s="144"/>
-      <c r="Q29" s="145"/>
+      <c r="N29" s="155"/>
+      <c r="O29" s="155"/>
+      <c r="P29" s="155"/>
+      <c r="Q29" s="156"/>
     </row>
     <row r="30" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="106"/>
@@ -7014,23 +7196,23 @@
       <c r="I30" s="107"/>
       <c r="J30" s="107"/>
       <c r="K30" s="108"/>
-      <c r="M30" s="146"/>
-      <c r="N30" s="147"/>
-      <c r="O30" s="147"/>
-      <c r="P30" s="147"/>
-      <c r="Q30" s="148"/>
+      <c r="M30" s="157"/>
+      <c r="N30" s="158"/>
+      <c r="O30" s="158"/>
+      <c r="P30" s="158"/>
+      <c r="Q30" s="159"/>
     </row>
     <row r="31" spans="4:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="153" t="s">
+      <c r="D31" s="149" t="s">
         <v>170</v>
       </c>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="154"/>
-      <c r="J31" s="154"/>
-      <c r="K31" s="155"/>
+      <c r="E31" s="150"/>
+      <c r="F31" s="150"/>
+      <c r="G31" s="150"/>
+      <c r="H31" s="150"/>
+      <c r="I31" s="150"/>
+      <c r="J31" s="150"/>
+      <c r="K31" s="151"/>
       <c r="M31" s="109" t="s">
         <v>170</v>
       </c>
@@ -7055,170 +7237,170 @@
       <c r="Q32" s="105"/>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D33" s="141"/>
+      <c r="D33" s="143"/>
       <c r="E33" s="53"/>
       <c r="F33" s="54"/>
-      <c r="G33" s="141"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
+      <c r="G33" s="143"/>
+      <c r="H33" s="143"/>
+      <c r="I33" s="143"/>
       <c r="J33" s="82"/>
-      <c r="K33" s="141"/>
-      <c r="M33" s="141"/>
-      <c r="N33" s="141"/>
-      <c r="O33" s="141"/>
+      <c r="K33" s="143"/>
+      <c r="M33" s="143"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="143"/>
       <c r="P33" s="82"/>
-      <c r="Q33" s="141"/>
+      <c r="Q33" s="143"/>
     </row>
     <row r="34" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="142"/>
+      <c r="D34" s="144"/>
       <c r="E34" s="67"/>
       <c r="F34" s="52"/>
-      <c r="G34" s="142"/>
-      <c r="H34" s="142"/>
-      <c r="I34" s="142"/>
+      <c r="G34" s="144"/>
+      <c r="H34" s="144"/>
+      <c r="I34" s="144"/>
       <c r="J34" s="82"/>
-      <c r="K34" s="142"/>
-      <c r="M34" s="142"/>
-      <c r="N34" s="142"/>
-      <c r="O34" s="142"/>
+      <c r="K34" s="144"/>
+      <c r="M34" s="144"/>
+      <c r="N34" s="144"/>
+      <c r="O34" s="144"/>
       <c r="P34" s="82"/>
-      <c r="Q34" s="142"/>
+      <c r="Q34" s="144"/>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D35" s="141"/>
+      <c r="D35" s="143"/>
       <c r="E35" s="53"/>
       <c r="F35" s="54"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="141"/>
+      <c r="G35" s="143"/>
+      <c r="H35" s="143"/>
+      <c r="I35" s="143"/>
       <c r="J35" s="82"/>
-      <c r="K35" s="141"/>
-      <c r="M35" s="141"/>
-      <c r="N35" s="141"/>
-      <c r="O35" s="141"/>
+      <c r="K35" s="143"/>
+      <c r="M35" s="143"/>
+      <c r="N35" s="143"/>
+      <c r="O35" s="143"/>
       <c r="P35" s="82"/>
-      <c r="Q35" s="141"/>
+      <c r="Q35" s="143"/>
     </row>
     <row r="36" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="142"/>
+      <c r="D36" s="144"/>
       <c r="E36" s="67"/>
       <c r="F36" s="52"/>
-      <c r="G36" s="142"/>
-      <c r="H36" s="142"/>
-      <c r="I36" s="142"/>
+      <c r="G36" s="144"/>
+      <c r="H36" s="144"/>
+      <c r="I36" s="144"/>
       <c r="J36" s="82"/>
-      <c r="K36" s="142"/>
-      <c r="M36" s="142"/>
-      <c r="N36" s="142"/>
-      <c r="O36" s="142"/>
+      <c r="K36" s="144"/>
+      <c r="M36" s="144"/>
+      <c r="N36" s="144"/>
+      <c r="O36" s="144"/>
       <c r="P36" s="82"/>
-      <c r="Q36" s="142"/>
+      <c r="Q36" s="144"/>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D37" s="141"/>
+      <c r="D37" s="143"/>
       <c r="E37" s="53"/>
       <c r="F37" s="54"/>
-      <c r="G37" s="141"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="141"/>
+      <c r="G37" s="143"/>
+      <c r="H37" s="143"/>
+      <c r="I37" s="143"/>
       <c r="J37" s="82"/>
-      <c r="K37" s="141"/>
-      <c r="M37" s="141"/>
-      <c r="N37" s="141"/>
-      <c r="O37" s="141"/>
+      <c r="K37" s="143"/>
+      <c r="M37" s="143"/>
+      <c r="N37" s="143"/>
+      <c r="O37" s="143"/>
       <c r="P37" s="82"/>
-      <c r="Q37" s="141"/>
+      <c r="Q37" s="143"/>
     </row>
     <row r="38" spans="4:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="142"/>
+      <c r="D38" s="144"/>
       <c r="E38" s="67"/>
       <c r="F38" s="52"/>
-      <c r="G38" s="142"/>
-      <c r="H38" s="142"/>
-      <c r="I38" s="142"/>
+      <c r="G38" s="144"/>
+      <c r="H38" s="144"/>
+      <c r="I38" s="144"/>
       <c r="J38" s="82"/>
-      <c r="K38" s="142"/>
-      <c r="M38" s="142"/>
-      <c r="N38" s="142"/>
-      <c r="O38" s="142"/>
+      <c r="K38" s="144"/>
+      <c r="M38" s="144"/>
+      <c r="N38" s="144"/>
+      <c r="O38" s="144"/>
       <c r="P38" s="82"/>
-      <c r="Q38" s="142"/>
+      <c r="Q38" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="K33:K34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="N37:N38"/>
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="Q37:Q38"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="N33:N34"/>
+    <mergeCell ref="O33:O34"/>
+    <mergeCell ref="Q33:Q34"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="O35:O36"/>
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="M29:Q30"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="Q27:Q28"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="N23:N24"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="M17:M18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="P15:P16"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="D31:K31"/>
     <mergeCell ref="D29:K29"/>
@@ -7243,79 +7425,79 @@
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="J21:J22"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="P15:P16"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="M17:M18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="N23:N24"/>
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="M29:Q30"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="N37:N38"/>
-    <mergeCell ref="O37:O38"/>
-    <mergeCell ref="Q37:Q38"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="N33:N34"/>
-    <mergeCell ref="O33:O34"/>
-    <mergeCell ref="Q33:Q34"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="O35:O36"/>
-    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="K33:K34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7327,8 +7509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:I106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80:H106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7361,13 +7543,13 @@
       <c r="E5" s="90">
         <v>1</v>
       </c>
-      <c r="F5" s="159" t="s">
+      <c r="F5" s="164" t="s">
         <v>165</v>
       </c>
       <c r="G5" s="90">
         <v>512</v>
       </c>
-      <c r="H5" s="161" t="s">
+      <c r="H5" s="166" t="s">
         <v>166</v>
       </c>
       <c r="I5" s="101" t="s">
@@ -7375,99 +7557,99 @@
       </c>
     </row>
     <row r="6" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="160"/>
-      <c r="H6" s="162"/>
+      <c r="F6" s="165"/>
+      <c r="H6" s="167"/>
     </row>
     <row r="7" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F7" s="160"/>
-      <c r="H7" s="162"/>
+      <c r="F7" s="165"/>
+      <c r="H7" s="167"/>
     </row>
     <row r="8" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="160"/>
-      <c r="H8" s="162"/>
+      <c r="F8" s="165"/>
+      <c r="H8" s="167"/>
     </row>
     <row r="9" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="160"/>
-      <c r="H9" s="162"/>
+      <c r="F9" s="165"/>
+      <c r="H9" s="167"/>
     </row>
     <row r="10" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F10" s="160"/>
-      <c r="H10" s="162"/>
+      <c r="F10" s="165"/>
+      <c r="H10" s="167"/>
     </row>
     <row r="11" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F11" s="160"/>
-      <c r="H11" s="162"/>
+      <c r="F11" s="165"/>
+      <c r="H11" s="167"/>
     </row>
     <row r="12" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F12" s="160"/>
-      <c r="H12" s="162"/>
+      <c r="F12" s="165"/>
+      <c r="H12" s="167"/>
     </row>
     <row r="13" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F13" s="160"/>
-      <c r="H13" s="162"/>
+      <c r="F13" s="165"/>
+      <c r="H13" s="167"/>
     </row>
     <row r="14" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F14" s="160"/>
-      <c r="H14" s="162"/>
+      <c r="F14" s="165"/>
+      <c r="H14" s="167"/>
     </row>
     <row r="15" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F15" s="160"/>
-      <c r="H15" s="162"/>
+      <c r="F15" s="165"/>
+      <c r="H15" s="167"/>
     </row>
     <row r="16" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F16" s="160"/>
-      <c r="H16" s="162"/>
+      <c r="F16" s="165"/>
+      <c r="H16" s="167"/>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F17" s="99"/>
-      <c r="H17" s="162"/>
+      <c r="H17" s="167"/>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F18" s="99"/>
-      <c r="H18" s="162"/>
+      <c r="H18" s="167"/>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F19" s="99"/>
-      <c r="H19" s="162"/>
+      <c r="H19" s="167"/>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H20" s="162"/>
+      <c r="H20" s="167"/>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H21" s="162"/>
+      <c r="H21" s="167"/>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H22" s="162"/>
+      <c r="H22" s="167"/>
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H23" s="162"/>
+      <c r="H23" s="167"/>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="162"/>
+      <c r="H24" s="167"/>
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H25" s="162"/>
+      <c r="H25" s="167"/>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H26" s="162"/>
+      <c r="H26" s="167"/>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="162"/>
+      <c r="H27" s="167"/>
     </row>
     <row r="28" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H28" s="162"/>
+      <c r="H28" s="167"/>
     </row>
     <row r="29" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="162"/>
+      <c r="H29" s="167"/>
     </row>
     <row r="30" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="162"/>
+      <c r="H30" s="167"/>
     </row>
     <row r="31" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H31" s="162"/>
+      <c r="H31" s="167"/>
     </row>
     <row r="32" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H32" s="162"/>
+      <c r="H32" s="167"/>
     </row>
     <row r="33" spans="5:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H33" s="100"/>
@@ -7476,13 +7658,13 @@
       <c r="E34" s="90">
         <v>2</v>
       </c>
-      <c r="F34" s="158" t="s">
+      <c r="F34" s="163" t="s">
         <v>169</v>
       </c>
       <c r="G34" s="90">
         <v>451</v>
       </c>
-      <c r="H34" s="158" t="s">
+      <c r="H34" s="163" t="s">
         <v>168</v>
       </c>
       <c r="I34" s="101" t="s">
@@ -7490,88 +7672,88 @@
       </c>
     </row>
     <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F35" s="158"/>
-      <c r="H35" s="158"/>
+      <c r="F35" s="163"/>
+      <c r="H35" s="163"/>
     </row>
     <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F36" s="158"/>
-      <c r="H36" s="158"/>
+      <c r="F36" s="163"/>
+      <c r="H36" s="163"/>
     </row>
     <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F37" s="158"/>
-      <c r="H37" s="158"/>
+      <c r="F37" s="163"/>
+      <c r="H37" s="163"/>
     </row>
     <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F38" s="158"/>
-      <c r="H38" s="158"/>
+      <c r="F38" s="163"/>
+      <c r="H38" s="163"/>
     </row>
     <row r="39" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F39" s="158"/>
-      <c r="H39" s="158"/>
+      <c r="F39" s="163"/>
+      <c r="H39" s="163"/>
     </row>
     <row r="40" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F40" s="158"/>
-      <c r="H40" s="158"/>
+      <c r="F40" s="163"/>
+      <c r="H40" s="163"/>
     </row>
     <row r="41" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F41" s="158"/>
-      <c r="H41" s="158"/>
+      <c r="F41" s="163"/>
+      <c r="H41" s="163"/>
     </row>
     <row r="42" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F42" s="158"/>
-      <c r="H42" s="158"/>
+      <c r="F42" s="163"/>
+      <c r="H42" s="163"/>
     </row>
     <row r="43" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F43" s="158"/>
-      <c r="H43" s="158"/>
+      <c r="F43" s="163"/>
+      <c r="H43" s="163"/>
     </row>
     <row r="44" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F44" s="158"/>
-      <c r="H44" s="158"/>
+      <c r="F44" s="163"/>
+      <c r="H44" s="163"/>
     </row>
     <row r="45" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F45" s="100"/>
-      <c r="H45" s="158"/>
+      <c r="H45" s="163"/>
     </row>
     <row r="46" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F46" s="100"/>
-      <c r="H46" s="158"/>
+      <c r="H46" s="163"/>
     </row>
     <row r="47" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H47" s="158"/>
+      <c r="H47" s="163"/>
     </row>
     <row r="48" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H48" s="158"/>
+      <c r="H48" s="163"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H49" s="158"/>
+      <c r="H49" s="163"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H50" s="158"/>
+      <c r="H50" s="163"/>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="158"/>
+      <c r="H51" s="163"/>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="158"/>
+      <c r="H52" s="163"/>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H53" s="158"/>
+      <c r="H53" s="163"/>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H54" s="158"/>
+      <c r="H54" s="163"/>
     </row>
     <row r="55" spans="5:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E55" s="90">
         <v>3</v>
       </c>
-      <c r="F55" s="158" t="s">
+      <c r="F55" s="163" t="s">
         <v>171</v>
       </c>
       <c r="G55" s="90">
         <v>512</v>
       </c>
-      <c r="H55" s="158" t="s">
+      <c r="H55" s="163" t="s">
         <v>172</v>
       </c>
       <c r="I55" s="101" t="s">
@@ -7579,109 +7761,109 @@
       </c>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F56" s="158"/>
-      <c r="H56" s="158"/>
+      <c r="F56" s="163"/>
+      <c r="H56" s="163"/>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F57" s="158"/>
-      <c r="H57" s="158"/>
+      <c r="F57" s="163"/>
+      <c r="H57" s="163"/>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F58" s="158"/>
-      <c r="H58" s="158"/>
+      <c r="F58" s="163"/>
+      <c r="H58" s="163"/>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F59" s="158"/>
-      <c r="H59" s="158"/>
+      <c r="F59" s="163"/>
+      <c r="H59" s="163"/>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F60" s="158"/>
-      <c r="H60" s="158"/>
+      <c r="F60" s="163"/>
+      <c r="H60" s="163"/>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F61" s="158"/>
-      <c r="H61" s="158"/>
+      <c r="F61" s="163"/>
+      <c r="H61" s="163"/>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F62" s="158"/>
-      <c r="H62" s="158"/>
+      <c r="F62" s="163"/>
+      <c r="H62" s="163"/>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F63" s="158"/>
-      <c r="H63" s="158"/>
+      <c r="F63" s="163"/>
+      <c r="H63" s="163"/>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F64" s="158"/>
-      <c r="H64" s="158"/>
+      <c r="F64" s="163"/>
+      <c r="H64" s="163"/>
     </row>
     <row r="65" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F65" s="158"/>
-      <c r="H65" s="158"/>
+      <c r="F65" s="163"/>
+      <c r="H65" s="163"/>
     </row>
     <row r="66" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F66" s="158"/>
-      <c r="H66" s="158"/>
+      <c r="F66" s="163"/>
+      <c r="H66" s="163"/>
     </row>
     <row r="67" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F67" s="158"/>
-      <c r="H67" s="158"/>
+      <c r="F67" s="163"/>
+      <c r="H67" s="163"/>
     </row>
     <row r="68" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F68" s="158"/>
-      <c r="H68" s="158"/>
+      <c r="F68" s="163"/>
+      <c r="H68" s="163"/>
     </row>
     <row r="69" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F69" s="158"/>
-      <c r="H69" s="158"/>
+      <c r="F69" s="163"/>
+      <c r="H69" s="163"/>
     </row>
     <row r="70" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F70" s="158"/>
-      <c r="H70" s="158"/>
+      <c r="F70" s="163"/>
+      <c r="H70" s="163"/>
     </row>
     <row r="71" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F71" s="158"/>
-      <c r="H71" s="158"/>
+      <c r="F71" s="163"/>
+      <c r="H71" s="163"/>
     </row>
     <row r="72" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F72" s="158"/>
-      <c r="H72" s="158"/>
+      <c r="F72" s="163"/>
+      <c r="H72" s="163"/>
     </row>
     <row r="73" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F73" s="158"/>
-      <c r="H73" s="158"/>
+      <c r="F73" s="163"/>
+      <c r="H73" s="163"/>
     </row>
     <row r="74" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F74" s="158"/>
-      <c r="H74" s="158"/>
+      <c r="F74" s="163"/>
+      <c r="H74" s="163"/>
     </row>
     <row r="75" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F75" s="158"/>
-      <c r="H75" s="158"/>
+      <c r="F75" s="163"/>
+      <c r="H75" s="163"/>
     </row>
     <row r="76" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F76" s="158"/>
-      <c r="H76" s="158"/>
+      <c r="F76" s="163"/>
+      <c r="H76" s="163"/>
     </row>
     <row r="77" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H77" s="158"/>
+      <c r="H77" s="163"/>
     </row>
     <row r="78" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H78" s="158"/>
+      <c r="H78" s="163"/>
     </row>
     <row r="79" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H79" s="158"/>
+      <c r="H79" s="163"/>
     </row>
     <row r="80" spans="5:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E80" s="90">
         <v>4</v>
       </c>
-      <c r="F80" s="178" t="s">
+      <c r="F80" s="160" t="s">
         <v>179</v>
       </c>
       <c r="G80" s="90">
         <v>451</v>
       </c>
-      <c r="H80" s="179" t="s">
+      <c r="H80" s="162" t="s">
         <v>181</v>
       </c>
       <c r="I80" s="101" t="s">
@@ -7689,93 +7871,93 @@
       </c>
     </row>
     <row r="81" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F81" s="180"/>
-      <c r="H81" s="179"/>
+      <c r="F81" s="161"/>
+      <c r="H81" s="162"/>
     </row>
     <row r="82" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F82" s="180"/>
-      <c r="H82" s="179"/>
+      <c r="F82" s="161"/>
+      <c r="H82" s="162"/>
     </row>
     <row r="83" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F83" s="180"/>
-      <c r="H83" s="179"/>
+      <c r="F83" s="161"/>
+      <c r="H83" s="162"/>
     </row>
     <row r="84" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F84" s="180"/>
-      <c r="H84" s="179"/>
+      <c r="F84" s="161"/>
+      <c r="H84" s="162"/>
     </row>
     <row r="85" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F85" s="180"/>
-      <c r="H85" s="179"/>
+      <c r="F85" s="161"/>
+      <c r="H85" s="162"/>
     </row>
     <row r="86" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F86" s="180"/>
-      <c r="H86" s="179"/>
+      <c r="F86" s="161"/>
+      <c r="H86" s="162"/>
     </row>
     <row r="87" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F87" s="180"/>
-      <c r="H87" s="179"/>
+      <c r="F87" s="161"/>
+      <c r="H87" s="162"/>
     </row>
     <row r="88" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F88" s="180"/>
-      <c r="H88" s="179"/>
+      <c r="F88" s="161"/>
+      <c r="H88" s="162"/>
     </row>
     <row r="89" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F89" s="180"/>
-      <c r="H89" s="179"/>
+      <c r="F89" s="161"/>
+      <c r="H89" s="162"/>
     </row>
     <row r="90" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F90" s="180"/>
-      <c r="H90" s="179"/>
+      <c r="F90" s="161"/>
+      <c r="H90" s="162"/>
     </row>
     <row r="91" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F91" s="180"/>
-      <c r="H91" s="179"/>
+      <c r="F91" s="161"/>
+      <c r="H91" s="162"/>
     </row>
     <row r="92" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H92" s="179"/>
+      <c r="H92" s="162"/>
     </row>
     <row r="93" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H93" s="179"/>
+      <c r="H93" s="162"/>
     </row>
     <row r="94" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H94" s="179"/>
+      <c r="H94" s="162"/>
     </row>
     <row r="95" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H95" s="179"/>
+      <c r="H95" s="162"/>
     </row>
     <row r="96" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="H96" s="179"/>
+      <c r="H96" s="162"/>
     </row>
     <row r="97" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H97" s="179"/>
+      <c r="H97" s="162"/>
     </row>
     <row r="98" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H98" s="179"/>
+      <c r="H98" s="162"/>
     </row>
     <row r="99" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H99" s="179"/>
+      <c r="H99" s="162"/>
     </row>
     <row r="100" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H100" s="179"/>
+      <c r="H100" s="162"/>
     </row>
     <row r="101" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H101" s="179"/>
+      <c r="H101" s="162"/>
     </row>
     <row r="102" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H102" s="179"/>
+      <c r="H102" s="162"/>
     </row>
     <row r="103" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H103" s="179"/>
+      <c r="H103" s="162"/>
     </row>
     <row r="104" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H104" s="179"/>
+      <c r="H104" s="162"/>
     </row>
     <row r="105" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H105" s="179"/>
+      <c r="H105" s="162"/>
     </row>
     <row r="106" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H106" s="179"/>
+      <c r="H106" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -7797,8 +7979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:K110"/>
   <sheetViews>
-    <sheetView topLeftCell="B77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView topLeftCell="B100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7814,48 +7996,48 @@
   <sheetData>
     <row r="4" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="163">
+      <c r="D5" s="168">
         <f>F17</f>
         <v>0</v>
       </c>
-      <c r="E5" s="164"/>
-      <c r="F5" s="164"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
       <c r="G5" s="64">
         <v>0.42850694444444448</v>
       </c>
       <c r="H5" s="113"/>
     </row>
     <row r="6" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="172" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="168"/>
-      <c r="F6" s="169"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="174"/>
       <c r="G6" s="70">
         <v>97</v>
       </c>
       <c r="H6" s="113"/>
     </row>
     <row r="7" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="167" t="s">
+      <c r="D7" s="172" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="168"/>
-      <c r="F7" s="169"/>
+      <c r="E7" s="173"/>
+      <c r="F7" s="174"/>
       <c r="G7" s="71">
         <v>4</v>
       </c>
       <c r="H7" s="113"/>
     </row>
     <row r="8" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="167" t="s">
+      <c r="D8" s="172" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="169"/>
-      <c r="F8" s="170" t="s">
+      <c r="E8" s="174"/>
+      <c r="F8" s="175" t="s">
         <v>144</v>
       </c>
-      <c r="G8" s="171"/>
+      <c r="G8" s="176"/>
       <c r="H8" s="113"/>
     </row>
     <row r="9" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7896,13 +8078,13 @@
       <c r="D11" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="172"/>
-      <c r="F11" s="172"/>
-      <c r="G11" s="173"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="178"/>
     </row>
     <row r="12" spans="4:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="165"/>
-      <c r="E12" s="166"/>
+      <c r="D12" s="170"/>
+      <c r="E12" s="171"/>
       <c r="F12" s="77" t="s">
         <v>143</v>
       </c>
@@ -7931,13 +8113,13 @@
       <c r="D23" s="90">
         <v>1</v>
       </c>
-      <c r="E23" s="161" t="s">
+      <c r="E23" s="166" t="s">
         <v>165</v>
       </c>
       <c r="F23" s="90">
         <v>512</v>
       </c>
-      <c r="G23" s="161" t="s">
+      <c r="G23" s="166" t="s">
         <v>174</v>
       </c>
       <c r="H23" s="101" t="s">
@@ -7945,87 +8127,87 @@
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="162"/>
-      <c r="G24" s="162"/>
+      <c r="E24" s="167"/>
+      <c r="G24" s="167"/>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="162"/>
-      <c r="G25" s="162"/>
+      <c r="E25" s="167"/>
+      <c r="G25" s="167"/>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="162"/>
-      <c r="G26" s="162"/>
+      <c r="E26" s="167"/>
+      <c r="G26" s="167"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="162"/>
-      <c r="G27" s="162"/>
+      <c r="E27" s="167"/>
+      <c r="G27" s="167"/>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E28" s="162"/>
-      <c r="G28" s="162"/>
+      <c r="E28" s="167"/>
+      <c r="G28" s="167"/>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="162"/>
-      <c r="G29" s="162"/>
+      <c r="E29" s="167"/>
+      <c r="G29" s="167"/>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E30" s="162"/>
-      <c r="G30" s="162"/>
+      <c r="E30" s="167"/>
+      <c r="G30" s="167"/>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E31" s="162"/>
-      <c r="G31" s="162"/>
+      <c r="E31" s="167"/>
+      <c r="G31" s="167"/>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E32" s="162"/>
-      <c r="G32" s="162"/>
+      <c r="E32" s="167"/>
+      <c r="G32" s="167"/>
     </row>
     <row r="33" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="162"/>
-      <c r="G33" s="162"/>
+      <c r="E33" s="167"/>
+      <c r="G33" s="167"/>
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="162"/>
-      <c r="G34" s="162"/>
+      <c r="E34" s="167"/>
+      <c r="G34" s="167"/>
     </row>
     <row r="35" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G35" s="162"/>
+      <c r="G35" s="167"/>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G36" s="162"/>
+      <c r="G36" s="167"/>
     </row>
     <row r="37" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="162"/>
+      <c r="G37" s="167"/>
     </row>
     <row r="38" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G38" s="162"/>
+      <c r="G38" s="167"/>
     </row>
     <row r="39" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G39" s="162"/>
+      <c r="G39" s="167"/>
     </row>
     <row r="40" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G40" s="162"/>
+      <c r="G40" s="167"/>
     </row>
     <row r="41" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G41" s="162"/>
+      <c r="G41" s="167"/>
     </row>
     <row r="42" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G42" s="162"/>
+      <c r="G42" s="167"/>
     </row>
     <row r="43" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G43" s="162"/>
+      <c r="G43" s="167"/>
     </row>
     <row r="44" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D44" s="90">
         <v>2</v>
       </c>
-      <c r="E44" s="158" t="s">
+      <c r="E44" s="163" t="s">
         <v>169</v>
       </c>
       <c r="F44" s="90">
         <v>451</v>
       </c>
-      <c r="G44" s="162" t="s">
+      <c r="G44" s="167" t="s">
         <v>176</v>
       </c>
       <c r="H44" s="101" t="s">
@@ -8033,101 +8215,101 @@
       </c>
     </row>
     <row r="45" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E45" s="158"/>
-      <c r="G45" s="162"/>
+      <c r="E45" s="163"/>
+      <c r="G45" s="167"/>
     </row>
     <row r="46" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E46" s="158"/>
-      <c r="G46" s="162"/>
+      <c r="E46" s="163"/>
+      <c r="G46" s="167"/>
     </row>
     <row r="47" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E47" s="158"/>
-      <c r="G47" s="162"/>
+      <c r="E47" s="163"/>
+      <c r="G47" s="167"/>
     </row>
     <row r="48" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E48" s="158"/>
-      <c r="G48" s="162"/>
+      <c r="E48" s="163"/>
+      <c r="G48" s="167"/>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E49" s="158"/>
-      <c r="G49" s="162"/>
+      <c r="E49" s="163"/>
+      <c r="G49" s="167"/>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E50" s="158"/>
-      <c r="G50" s="162"/>
+      <c r="E50" s="163"/>
+      <c r="G50" s="167"/>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E51" s="158"/>
-      <c r="G51" s="162"/>
+      <c r="E51" s="163"/>
+      <c r="G51" s="167"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E52" s="158"/>
-      <c r="G52" s="162"/>
+      <c r="E52" s="163"/>
+      <c r="G52" s="167"/>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E53" s="158"/>
-      <c r="G53" s="162"/>
+      <c r="E53" s="163"/>
+      <c r="G53" s="167"/>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E54" s="158"/>
-      <c r="G54" s="162"/>
+      <c r="E54" s="163"/>
+      <c r="G54" s="167"/>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="162"/>
+      <c r="G55" s="167"/>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="162"/>
+      <c r="G56" s="167"/>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G57" s="162"/>
+      <c r="G57" s="167"/>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G58" s="162"/>
+      <c r="G58" s="167"/>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G59" s="162"/>
+      <c r="G59" s="167"/>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G60" s="162"/>
+      <c r="G60" s="167"/>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G61" s="162"/>
+      <c r="G61" s="167"/>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G62" s="162"/>
+      <c r="G62" s="167"/>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G63" s="162"/>
+      <c r="G63" s="167"/>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G64" s="162"/>
+      <c r="G64" s="167"/>
     </row>
     <row r="65" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G65" s="162"/>
+      <c r="G65" s="167"/>
     </row>
     <row r="66" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G66" s="162"/>
+      <c r="G66" s="167"/>
     </row>
     <row r="67" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G67" s="162"/>
+      <c r="G67" s="167"/>
     </row>
     <row r="68" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G68" s="162"/>
+      <c r="G68" s="167"/>
     </row>
     <row r="69" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G69" s="162"/>
+      <c r="G69" s="167"/>
     </row>
     <row r="70" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="90">
         <v>3</v>
       </c>
-      <c r="E70" s="158" t="s">
+      <c r="E70" s="163" t="s">
         <v>171</v>
       </c>
       <c r="F70" s="90">
         <v>512</v>
       </c>
-      <c r="G70" s="162" t="s">
+      <c r="G70" s="167" t="s">
         <v>177</v>
       </c>
       <c r="H70" s="101" t="s">
@@ -8135,115 +8317,115 @@
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E71" s="158"/>
-      <c r="G71" s="162"/>
+      <c r="E71" s="163"/>
+      <c r="G71" s="167"/>
     </row>
     <row r="72" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E72" s="158"/>
-      <c r="G72" s="162"/>
+      <c r="E72" s="163"/>
+      <c r="G72" s="167"/>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E73" s="158"/>
-      <c r="G73" s="162"/>
+      <c r="E73" s="163"/>
+      <c r="G73" s="167"/>
     </row>
     <row r="74" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E74" s="158"/>
-      <c r="G74" s="162"/>
+      <c r="E74" s="163"/>
+      <c r="G74" s="167"/>
     </row>
     <row r="75" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E75" s="158"/>
-      <c r="G75" s="162"/>
+      <c r="E75" s="163"/>
+      <c r="G75" s="167"/>
     </row>
     <row r="76" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E76" s="158"/>
-      <c r="G76" s="162"/>
+      <c r="E76" s="163"/>
+      <c r="G76" s="167"/>
     </row>
     <row r="77" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E77" s="158"/>
-      <c r="G77" s="162"/>
+      <c r="E77" s="163"/>
+      <c r="G77" s="167"/>
     </row>
     <row r="78" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E78" s="158"/>
-      <c r="G78" s="162"/>
+      <c r="E78" s="163"/>
+      <c r="G78" s="167"/>
     </row>
     <row r="79" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E79" s="158"/>
-      <c r="G79" s="162"/>
+      <c r="E79" s="163"/>
+      <c r="G79" s="167"/>
     </row>
     <row r="80" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E80" s="158"/>
-      <c r="G80" s="162"/>
+      <c r="E80" s="163"/>
+      <c r="G80" s="167"/>
     </row>
     <row r="81" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E81" s="158"/>
-      <c r="G81" s="162"/>
+      <c r="E81" s="163"/>
+      <c r="G81" s="167"/>
     </row>
     <row r="82" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E82" s="158"/>
-      <c r="G82" s="162"/>
+      <c r="E82" s="163"/>
+      <c r="G82" s="167"/>
     </row>
     <row r="83" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E83" s="158"/>
-      <c r="G83" s="162"/>
+      <c r="E83" s="163"/>
+      <c r="G83" s="167"/>
     </row>
     <row r="84" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E84" s="158"/>
-      <c r="G84" s="162"/>
+      <c r="E84" s="163"/>
+      <c r="G84" s="167"/>
     </row>
     <row r="85" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E85" s="158"/>
-      <c r="G85" s="162"/>
+      <c r="E85" s="163"/>
+      <c r="G85" s="167"/>
     </row>
     <row r="86" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E86" s="158"/>
-      <c r="G86" s="162"/>
+      <c r="E86" s="163"/>
+      <c r="G86" s="167"/>
     </row>
     <row r="87" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E87" s="158"/>
-      <c r="G87" s="162"/>
+      <c r="E87" s="163"/>
+      <c r="G87" s="167"/>
     </row>
     <row r="88" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E88" s="158"/>
-      <c r="G88" s="162"/>
+      <c r="E88" s="163"/>
+      <c r="G88" s="167"/>
     </row>
     <row r="89" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E89" s="158"/>
-      <c r="G89" s="162"/>
+      <c r="E89" s="163"/>
+      <c r="G89" s="167"/>
     </row>
     <row r="90" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E90" s="158"/>
-      <c r="G90" s="162"/>
+      <c r="E90" s="163"/>
+      <c r="G90" s="167"/>
     </row>
     <row r="91" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E91" s="158"/>
-      <c r="G91" s="162"/>
+      <c r="E91" s="163"/>
+      <c r="G91" s="167"/>
     </row>
     <row r="92" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="162"/>
+      <c r="G92" s="167"/>
     </row>
     <row r="93" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G93" s="162"/>
+      <c r="G93" s="167"/>
     </row>
     <row r="94" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G94" s="162"/>
+      <c r="G94" s="167"/>
     </row>
     <row r="95" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G95" s="162"/>
+      <c r="G95" s="167"/>
     </row>
     <row r="96" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G96" s="162"/>
+      <c r="G96" s="167"/>
     </row>
     <row r="97" spans="4:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D97" s="90">
         <v>4</v>
       </c>
-      <c r="E97" s="178" t="s">
+      <c r="E97" s="160" t="s">
         <v>179</v>
       </c>
       <c r="F97" s="90">
         <v>451</v>
       </c>
-      <c r="G97" s="158" t="s">
+      <c r="G97" s="163" t="s">
         <v>180</v>
       </c>
       <c r="H97" s="101" t="s">
@@ -8251,54 +8433,54 @@
       </c>
     </row>
     <row r="98" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E98" s="180"/>
-      <c r="G98" s="158"/>
+      <c r="E98" s="161"/>
+      <c r="G98" s="163"/>
     </row>
     <row r="99" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E99" s="180"/>
-      <c r="G99" s="158"/>
+      <c r="E99" s="161"/>
+      <c r="G99" s="163"/>
     </row>
     <row r="100" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E100" s="180"/>
-      <c r="G100" s="158"/>
+      <c r="E100" s="161"/>
+      <c r="G100" s="163"/>
     </row>
     <row r="101" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E101" s="180"/>
-      <c r="G101" s="158"/>
+      <c r="E101" s="161"/>
+      <c r="G101" s="163"/>
     </row>
     <row r="102" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E102" s="180"/>
-      <c r="G102" s="158"/>
+      <c r="E102" s="161"/>
+      <c r="G102" s="163"/>
     </row>
     <row r="103" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E103" s="180"/>
-      <c r="G103" s="158"/>
+      <c r="E103" s="161"/>
+      <c r="G103" s="163"/>
     </row>
     <row r="104" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E104" s="180"/>
-      <c r="G104" s="158"/>
+      <c r="E104" s="161"/>
+      <c r="G104" s="163"/>
     </row>
     <row r="105" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E105" s="180"/>
-      <c r="G105" s="158"/>
+      <c r="E105" s="161"/>
+      <c r="G105" s="163"/>
     </row>
     <row r="106" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E106" s="180"/>
-      <c r="G106" s="158"/>
+      <c r="E106" s="161"/>
+      <c r="G106" s="163"/>
     </row>
     <row r="107" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E107" s="180"/>
-      <c r="G107" s="158"/>
+      <c r="E107" s="161"/>
+      <c r="G107" s="163"/>
     </row>
     <row r="108" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E108" s="180"/>
-      <c r="G108" s="158"/>
+      <c r="E108" s="161"/>
+      <c r="G108" s="163"/>
     </row>
     <row r="109" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G109" s="158"/>
+      <c r="G109" s="163"/>
     </row>
     <row r="110" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="G110" s="158"/>
+      <c r="G110" s="163"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -8328,7 +8510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F5:Y482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="O10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -8350,10 +8532,10 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="I6" s="174" t="s">
+      <c r="I6" s="179" t="s">
         <v>141</v>
       </c>
-      <c r="J6" s="175"/>
+      <c r="J6" s="180"/>
       <c r="K6" s="31" t="s">
         <v>139</v>
       </c>
@@ -8377,8 +8559,8 @@
       <c r="F7">
         <v>5</v>
       </c>
-      <c r="I7" s="176"/>
-      <c r="J7" s="177"/>
+      <c r="I7" s="181"/>
+      <c r="J7" s="182"/>
       <c r="K7" s="22" t="s">
         <v>140</v>
       </c>
@@ -8424,19 +8606,19 @@
       <c r="F10" t="s">
         <v>137</v>
       </c>
-      <c r="U10" s="182" t="s">
+      <c r="U10" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="V10" s="181">
+      <c r="V10" s="115">
         <v>4.0355696145620703</v>
       </c>
-      <c r="W10" s="181">
+      <c r="W10" s="115">
         <v>4.25710743005782</v>
       </c>
-      <c r="X10" s="181">
+      <c r="X10" s="115">
         <v>3.77391380004984</v>
       </c>
-      <c r="Y10" s="181">
+      <c r="Y10" s="115">
         <v>4.4210870761961996</v>
       </c>
     </row>
@@ -8444,19 +8626,19 @@
       <c r="F11" t="s">
         <v>137</v>
       </c>
-      <c r="U11" s="182" t="s">
+      <c r="U11" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="V11" s="181">
+      <c r="V11" s="115">
         <v>4.0355696145620703</v>
       </c>
-      <c r="W11" s="181">
+      <c r="W11" s="115">
         <v>4.25710743005782</v>
       </c>
-      <c r="X11" s="181">
+      <c r="X11" s="115">
         <v>3.77391380004984</v>
       </c>
-      <c r="Y11" s="181">
+      <c r="Y11" s="115">
         <v>4.4210870761961996</v>
       </c>
     </row>
@@ -8522,16 +8704,16 @@
       <c r="P19" t="s">
         <v>185</v>
       </c>
-      <c r="Q19" s="181" t="s">
+      <c r="Q19" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="R19" s="181" t="s">
+      <c r="R19" s="115" t="s">
         <v>167</v>
       </c>
-      <c r="S19" s="181" t="s">
+      <c r="S19" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="T19" s="181" t="s">
+      <c r="T19" s="115" t="s">
         <v>178</v>
       </c>
     </row>
@@ -8542,16 +8724,16 @@
       <c r="P20" t="s">
         <v>186</v>
       </c>
-      <c r="Q20" s="181" t="s">
+      <c r="Q20" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="R20" s="181" t="s">
+      <c r="R20" s="115" t="s">
         <v>167</v>
       </c>
-      <c r="S20" s="181" t="s">
+      <c r="S20" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="T20" s="181" t="s">
+      <c r="T20" s="115" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>